<commit_message>
adding info about params
</commit_message>
<xml_diff>
--- a/parameters/Bevacizumab_model G parameters_VEGFR1.xlsx
+++ b/parameters/Bevacizumab_model G parameters_VEGFR1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/GitHub/TMDD_EndogenousLigand/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A93D2A-B232-914A-8730-1B775A20A368}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CDCC6A-8E17-5249-8F91-EAC3CA912F04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27:F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -861,7 +861,7 @@
         <v>86</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -898,7 +898,7 @@
         <v>87</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>